<commit_message>
Neuron study in depth
</commit_message>
<xml_diff>
--- a/1_ML_Combined_Courses/Practice/4_Excel/2_Simple_Neurons.xlsx
+++ b/1_ML_Combined_Courses/Practice/4_Excel/2_Simple_Neurons.xlsx
@@ -8,14 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\1_ML_Combined_Courses\Practice\4_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090CC851-84C5-43E2-B9B4-533B26FE14E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182491B3-8BC9-40C0-ABBB-888208527554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{BEFB4AB8-46B2-4D36-AF54-8C400EF49FEA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{BEFB4AB8-46B2-4D36-AF54-8C400EF49FEA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Eqn" sheetId="1" r:id="rId1"/>
+    <sheet name="Visual" sheetId="2" r:id="rId2"/>
+    <sheet name="Visual-2" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="w_1">'Visual-2'!$H$6</definedName>
+    <definedName name="w_2">'Visual-2'!$H$10</definedName>
+    <definedName name="w_3">'Visual-2'!$F$12</definedName>
+    <definedName name="w_4">'Visual-2'!$E$15</definedName>
+    <definedName name="w_5">'Visual-2'!$H$17</definedName>
+    <definedName name="w_6">'Visual-2'!$N$6</definedName>
+    <definedName name="w_7">'Visual-2'!$M$10</definedName>
+    <definedName name="w_8">'Visual-2'!$N$14</definedName>
+    <definedName name="x_0">'Visual-2'!$D$4</definedName>
+    <definedName name="x_1">'Visual-2'!$D$9</definedName>
+    <definedName name="x_2">'Visual-2'!$D$16</definedName>
+    <definedName name="z_1">'Visual-2'!$K$9</definedName>
+    <definedName name="z_2">'Visual-2'!$K$16</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>Base Equation</t>
   </si>
@@ -82,15 +98,45 @@
   <si>
     <t>y</t>
   </si>
+  <si>
+    <t>z1</t>
+  </si>
+  <si>
+    <t>z2</t>
+  </si>
+  <si>
+    <t>w4</t>
+  </si>
+  <si>
+    <t>w5</t>
+  </si>
+  <si>
+    <t>w6</t>
+  </si>
+  <si>
+    <t>w7</t>
+  </si>
+  <si>
+    <t>w8</t>
+  </si>
+  <si>
+    <t>Inputs</t>
+  </si>
+  <si>
+    <t>BIAS</t>
+  </si>
+  <si>
+    <t>Mid-layer</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,8 +205,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +267,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -242,9 +300,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -297,6 +355,39 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -820,6 +911,903 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Oval 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D045ACCB-FB40-4DA3-9040-F84ECA20C301}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1181100" y="238125"/>
+          <a:ext cx="657225" cy="657225"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Oval 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E45093F-99A8-4D8D-9A7F-8693C5C3CC7E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1143000" y="1371600"/>
+          <a:ext cx="657225" cy="657225"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Oval 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{048BA367-A747-4C12-9050-E4FA4531CB05}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1123950" y="3057525"/>
+          <a:ext cx="657225" cy="657225"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>109538</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>109538</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{800C0B66-C7DB-4829-9247-01A551F8CCE4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="2" idx="6"/>
+          <a:endCxn id="16" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1838325" y="566738"/>
+          <a:ext cx="2428875" cy="1143000"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>100013</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>109538</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25A12255-B3B5-4934-8FB3-2F1AA399B1A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="3" idx="6"/>
+          <a:endCxn id="16" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1800225" y="1700213"/>
+          <a:ext cx="2466975" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>138113</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>185738</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85020F20-F0A8-48F8-98F8-FC2D823F5391}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="4" idx="6"/>
+          <a:endCxn id="17" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1781175" y="3367088"/>
+          <a:ext cx="2524125" cy="47625"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Oval 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC633A5E-7265-40B2-9CFD-762B614B74EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4267200" y="1381125"/>
+          <a:ext cx="657225" cy="657225"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="0070C0"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="accent2"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Oval 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A284776D-8CF8-4FEC-AB50-FB42A8F7D8E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4305300" y="3019425"/>
+          <a:ext cx="752475" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="0070C0"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="accent2"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Oval 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8706740-D13C-4DAF-8B03-7DD4DB8CB8D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4248150" y="276225"/>
+          <a:ext cx="657225" cy="657225"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="0070C0"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="accent2"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>138113</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Straight Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{929C7997-CB33-42A4-BF93-F3F598D77C94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="3" idx="6"/>
+          <a:endCxn id="17" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1800225" y="1714500"/>
+          <a:ext cx="2505075" cy="1652588"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>171847</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="Oval 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18DCB339-BDAB-4B67-BFEC-E7C842B69201}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7019925" y="1314449"/>
+          <a:ext cx="848122" cy="838201"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="accent2"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>147638</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Straight Connector 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28325AAD-52AA-4469-BE91-CC16BDC732D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="21" idx="6"/>
+          <a:endCxn id="27" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5000625" y="604838"/>
+          <a:ext cx="2019300" cy="1128712"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Straight Connector 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EDF62A1-CA14-4A89-8DEA-5F8BA9AD2E6A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="16" idx="6"/>
+          <a:endCxn id="27" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5019675" y="1724025"/>
+          <a:ext cx="2000250" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>138113</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Straight Connector 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C8AD048-73A1-4F36-A27B-104DBCB65DE4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="17" idx="6"/>
+          <a:endCxn id="27" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5057775" y="1733550"/>
+          <a:ext cx="1962150" cy="1633538"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>109538</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>185738</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Straight Connector 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EEEE79F-E09A-42DD-B99D-F37203E41AC1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="4" idx="6"/>
+          <a:endCxn id="16" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1781175" y="1709738"/>
+          <a:ext cx="2486025" cy="1676400"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1243,7 +2231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B9E158D-22C4-4E13-AB0E-226916541DD8}">
   <dimension ref="B4:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
@@ -1312,4 +2300,181 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC2018B1-23CC-47EA-AD13-5345813D695F}">
+  <dimension ref="C1:R17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="5.625" style="13"/>
+    <col min="4" max="4" width="5.625" style="12"/>
+    <col min="5" max="7" width="5.625" style="13"/>
+    <col min="8" max="8" width="6.875" style="19" customWidth="1"/>
+    <col min="9" max="10" width="5.625" style="13"/>
+    <col min="11" max="11" width="6.875" style="19" customWidth="1"/>
+    <col min="12" max="12" width="5.625" style="13"/>
+    <col min="13" max="13" width="5.875" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.625" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="5.625" style="13"/>
+    <col min="17" max="17" width="7.25" style="13" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="5.625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C1" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="32"/>
+      <c r="H1" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="30"/>
+      <c r="Q1" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" s="30"/>
+    </row>
+    <row r="4" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C4" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="14">
+        <v>1</v>
+      </c>
+      <c r="K4" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="H5" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="H6" s="17">
+        <v>-1.5</v>
+      </c>
+      <c r="N6" s="17">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="K7" s="26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="K8" s="27"/>
+      <c r="Q8" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="3:18" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C9" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="14">
+        <v>0</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="28">
+        <f>x_0*w_1+x_1*w_2+x_2*w_4</f>
+        <v>-1.5</v>
+      </c>
+      <c r="L9" s="22"/>
+      <c r="M9" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q9" s="29">
+        <f>K4*w_6+z_1*w_7+z_2*w_8</f>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="10" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C10" s="21"/>
+      <c r="H10" s="17">
+        <v>1</v>
+      </c>
+      <c r="K10" s="27"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C11" s="21"/>
+      <c r="F11" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" s="27"/>
+      <c r="L11" s="22"/>
+    </row>
+    <row r="12" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C12" s="21"/>
+      <c r="F12" s="17">
+        <v>1</v>
+      </c>
+      <c r="K12" s="27"/>
+    </row>
+    <row r="13" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="K13" s="27"/>
+      <c r="N13" s="18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="E14" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="N14" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="E15" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C16" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="14">
+        <v>0</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="K16" s="28">
+        <f>x_1*w_3+x_2*w_5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="24">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
In-depth study and preparation of Truth table - Deep learning
</commit_message>
<xml_diff>
--- a/1_ML_Combined_Courses/Practice/4_Excel/2_Simple_Neurons.xlsx
+++ b/1_ML_Combined_Courses/Practice/4_Excel/2_Simple_Neurons.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\1_ML_Combined_Courses\Practice\4_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182491B3-8BC9-40C0-ABBB-888208527554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC1A4ED-EDE4-4192-AC03-BA1DA3C678A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{BEFB4AB8-46B2-4D36-AF54-8C400EF49FEA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{BEFB4AB8-46B2-4D36-AF54-8C400EF49FEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Eqn" sheetId="1" r:id="rId1"/>
     <sheet name="Visual" sheetId="2" r:id="rId2"/>
     <sheet name="Visual-2" sheetId="3" r:id="rId3"/>
+    <sheet name="Truth_Table" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="w_1">'Visual-2'!$H$6</definedName>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
   <si>
     <t>Base Equation</t>
   </si>
@@ -127,6 +128,69 @@
   </si>
   <si>
     <t>Mid-layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w0 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">w1 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">w2 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">w11 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">w12 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">w21 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">w22 = </t>
+  </si>
+  <si>
+    <t>z0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wz = </t>
+  </si>
+  <si>
+    <t>y =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wz1 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">wz2 = </t>
+  </si>
+  <si>
+    <t>x1 AND x2 AND (NOT x3)</t>
+  </si>
+  <si>
+    <t>z1_t</t>
+  </si>
+  <si>
+    <t>x1 AND x2</t>
+  </si>
+  <si>
+    <t>z2_t</t>
+  </si>
+  <si>
+    <t>(NOT x1) AND (NOT x2)</t>
+  </si>
+  <si>
+    <t>y_t</t>
+  </si>
+  <si>
+    <t>z1 OR z2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z1_b = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">y_b = </t>
   </si>
 </sst>
 </file>
@@ -136,7 +200,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,8 +275,70 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="8" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF002060"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -273,6 +399,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -302,7 +434,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -388,12 +520,134 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFFFF00"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFFFF00"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1808,6 +2062,72 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>392130</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F314F68B-8115-1853-05FE-ABAB545BF9D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4781550" y="171450"/>
+          <a:ext cx="4164030" cy="1819275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2304,10 +2624,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC2018B1-23CC-47EA-AD13-5345813D695F}">
-  <dimension ref="C1:R17"/>
+  <dimension ref="B1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -2467,14 +2787,710 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="H17" s="24">
         <v>1</v>
       </c>
+    </row>
+    <row r="20" spans="2:13" s="33" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B20" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="36">
+        <v>1</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="37">
+        <v>-1.5</v>
+      </c>
+      <c r="G20" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" s="36">
+        <v>1</v>
+      </c>
+      <c r="I20" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="J20" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" s="33" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="34"/>
+      <c r="I21" s="41"/>
+    </row>
+    <row r="22" spans="2:13" s="33" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="35"/>
+      <c r="I22" s="41"/>
+    </row>
+    <row r="23" spans="2:13" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="36">
+        <v>1</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="37">
+        <v>1</v>
+      </c>
+      <c r="G23" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="36">
+        <f>C20*E20+C23*E23+C26*E26</f>
+        <v>0.5</v>
+      </c>
+      <c r="I23" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="J23" s="37">
+        <v>1</v>
+      </c>
+      <c r="L23" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="M23" s="38">
+        <f>H20*J20+H23*J23+H26*J26</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" s="33" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="37">
+        <v>1</v>
+      </c>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="41"/>
+    </row>
+    <row r="25" spans="2:13" s="33" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="35"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="41"/>
+    </row>
+    <row r="26" spans="2:13" s="33" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B26" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="36">
+        <v>1</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="37">
+        <v>1</v>
+      </c>
+      <c r="G26" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" s="36">
+        <f>C23*E24+C26*E27</f>
+        <v>2</v>
+      </c>
+      <c r="I26" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="J26" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" s="33" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" s="37">
+        <v>1</v>
+      </c>
+      <c r="I27" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8968D895-8ACC-473E-B462-3A83C58DD586}">
+  <dimension ref="B1:U20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.625" style="33" customWidth="1"/>
+    <col min="2" max="3" width="7.625" style="34" customWidth="1"/>
+    <col min="4" max="5" width="7.625" style="33" customWidth="1"/>
+    <col min="6" max="6" width="22.875" style="33" customWidth="1"/>
+    <col min="7" max="19" width="5.625" style="33"/>
+    <col min="20" max="20" width="2.875" style="33" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.875" style="33" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="5.625" style="33"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B1" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="55">
+        <v>1</v>
+      </c>
+      <c r="D1" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="55">
+        <v>1</v>
+      </c>
+      <c r="F1" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="57">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="2" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B2" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="R2" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="T2" s="49" t="s">
+        <v>13</v>
+      </c>
+      <c r="U2" s="49" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B3" s="45">
+        <v>0</v>
+      </c>
+      <c r="C3" s="45">
+        <v>0</v>
+      </c>
+      <c r="D3" s="46">
+        <f>$G$1+B3*$C$1+C3*$E$1</f>
+        <v>-1.5</v>
+      </c>
+      <c r="E3" s="47">
+        <f>IF(D3&lt;0,0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="46">
+        <f>AND(B3,C3)*1</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="33" t="str">
+        <f>IF(E3=F3,"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="R3" s="50">
+        <v>0</v>
+      </c>
+      <c r="S3" s="50">
+        <v>0</v>
+      </c>
+      <c r="T3" s="50">
+        <v>0</v>
+      </c>
+      <c r="U3" s="51">
+        <f>AND(R3,S3,NOT(T3))*1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B4" s="45">
+        <v>0</v>
+      </c>
+      <c r="C4" s="45">
+        <v>1</v>
+      </c>
+      <c r="D4" s="46">
+        <f>$G$1+B4*$C$1+C4*$E$1</f>
+        <v>-0.5</v>
+      </c>
+      <c r="E4" s="47">
+        <f>IF(D4&lt;0,0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="46">
+        <f>AND(B4,C4)*1</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="33" t="str">
+        <f>IF(E4=F4,"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="R4" s="50">
+        <v>0</v>
+      </c>
+      <c r="S4" s="50">
+        <v>0</v>
+      </c>
+      <c r="T4" s="50">
+        <v>1</v>
+      </c>
+      <c r="U4" s="51">
+        <f t="shared" ref="U4:U10" si="0">AND(R4,S4,NOT(T4))*1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B5" s="45">
+        <v>1</v>
+      </c>
+      <c r="C5" s="45">
+        <v>0</v>
+      </c>
+      <c r="D5" s="46">
+        <f>$G$1+B5*$C$1+C5*$E$1</f>
+        <v>-0.5</v>
+      </c>
+      <c r="E5" s="47">
+        <f>IF(D5&lt;0,0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="46">
+        <f>AND(B5,C5)*1</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="33" t="str">
+        <f>IF(E5=F5,"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="R5" s="50">
+        <v>0</v>
+      </c>
+      <c r="S5" s="50">
+        <v>1</v>
+      </c>
+      <c r="T5" s="50">
+        <v>0</v>
+      </c>
+      <c r="U5" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B6" s="45">
+        <v>1</v>
+      </c>
+      <c r="C6" s="45">
+        <v>1</v>
+      </c>
+      <c r="D6" s="46">
+        <f>$G$1+B6*$C$1+C6*$E$1</f>
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="47">
+        <f>IF(D6&lt;0,0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="46">
+        <f>AND(B6,C6)*1</f>
+        <v>1</v>
+      </c>
+      <c r="G6" s="33" t="str">
+        <f>IF(E6=F6,"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="R6" s="50">
+        <v>0</v>
+      </c>
+      <c r="S6" s="50">
+        <v>1</v>
+      </c>
+      <c r="T6" s="50">
+        <v>1</v>
+      </c>
+      <c r="U6" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="43"/>
+      <c r="R7" s="50">
+        <v>1</v>
+      </c>
+      <c r="S7" s="50">
+        <v>0</v>
+      </c>
+      <c r="T7" s="50">
+        <v>0</v>
+      </c>
+      <c r="U7" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B8" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="55">
+        <v>-1</v>
+      </c>
+      <c r="D8" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="55">
+        <v>-1</v>
+      </c>
+      <c r="F8" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="57">
+        <v>1.5</v>
+      </c>
+      <c r="R8" s="50">
+        <v>1</v>
+      </c>
+      <c r="S8" s="50">
+        <v>0</v>
+      </c>
+      <c r="T8" s="50">
+        <v>1</v>
+      </c>
+      <c r="U8" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B9" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="R9" s="50">
+        <v>1</v>
+      </c>
+      <c r="S9" s="50">
+        <v>1</v>
+      </c>
+      <c r="T9" s="50">
+        <v>0</v>
+      </c>
+      <c r="U9" s="51">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B10" s="45">
+        <v>0</v>
+      </c>
+      <c r="C10" s="45">
+        <v>0</v>
+      </c>
+      <c r="D10" s="46">
+        <f>$G$8+B10*$C$8+C10*$E$8</f>
+        <v>1.5</v>
+      </c>
+      <c r="E10" s="47">
+        <f>IF(D10&lt;0,0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="F10" s="46">
+        <f>AND(NOT(B10),NOT(C10))*1</f>
+        <v>1</v>
+      </c>
+      <c r="G10" s="33" t="str">
+        <f>IF(E10=F10,"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="R10" s="50">
+        <v>1</v>
+      </c>
+      <c r="S10" s="50">
+        <v>1</v>
+      </c>
+      <c r="T10" s="50">
+        <v>1</v>
+      </c>
+      <c r="U10" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B11" s="45">
+        <v>0</v>
+      </c>
+      <c r="C11" s="45">
+        <v>1</v>
+      </c>
+      <c r="D11" s="46">
+        <f>$G$8+B11*$C$8+C11*$E$8</f>
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="47">
+        <f>IF(D11&lt;0,0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="F11" s="46">
+        <f>AND(NOT(B11),NOT(C11))*1</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="33" t="str">
+        <f>IF(E11=F11,"Y","N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B12" s="45">
+        <v>1</v>
+      </c>
+      <c r="C12" s="45">
+        <v>0</v>
+      </c>
+      <c r="D12" s="46">
+        <f>$G$8+B12*$C$8+C12*$E$8</f>
+        <v>0.5</v>
+      </c>
+      <c r="E12" s="47">
+        <f>IF(D12&lt;0,0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="F12" s="46">
+        <f>AND(NOT(B12),NOT(C12))*1</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="33" t="str">
+        <f>IF(E12=F12,"Y","N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B13" s="45">
+        <v>1</v>
+      </c>
+      <c r="C13" s="45">
+        <v>1</v>
+      </c>
+      <c r="D13" s="46">
+        <f>$G$8+B13*$C$8+C13*$E$8</f>
+        <v>-0.5</v>
+      </c>
+      <c r="E13" s="47">
+        <f>IF(D13&lt;0,0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="46">
+        <f>AND(NOT(B13),NOT(C13))*1</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="33" t="str">
+        <f>IF(E13=F13,"Y","N")</f>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="53"/>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B15" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="55">
+        <v>1</v>
+      </c>
+      <c r="D15" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="55">
+        <v>1</v>
+      </c>
+      <c r="F15" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="57">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B16" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="48" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="45">
+        <v>0</v>
+      </c>
+      <c r="C17" s="45">
+        <v>0</v>
+      </c>
+      <c r="D17" s="46">
+        <f>$G$15+B17*$C$15+C17*$E$15</f>
+        <v>-1.5</v>
+      </c>
+      <c r="E17" s="47">
+        <f>IF(D17&lt;0,0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="46">
+        <f>OR(B17,C17)*1</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="33" t="str">
+        <f>IF(E17=F17,"Y","N")</f>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="45">
+        <v>0</v>
+      </c>
+      <c r="C18" s="45">
+        <v>1</v>
+      </c>
+      <c r="D18" s="46">
+        <f>$G$15+B18*$C$15+C18*$E$15</f>
+        <v>-0.5</v>
+      </c>
+      <c r="E18" s="47">
+        <f>IF(D18&lt;0,0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="46">
+        <f>OR(B18,C18)*1</f>
+        <v>1</v>
+      </c>
+      <c r="G18" s="33" t="str">
+        <f>IF(E18=F18,"Y","N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="45">
+        <v>1</v>
+      </c>
+      <c r="C19" s="45">
+        <v>0</v>
+      </c>
+      <c r="D19" s="46">
+        <f>$G$15+B19*$C$15+C19*$E$15</f>
+        <v>-0.5</v>
+      </c>
+      <c r="E19" s="47">
+        <f>IF(D19&lt;0,0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="46">
+        <f>OR(B19,C19)*1</f>
+        <v>1</v>
+      </c>
+      <c r="G19" s="33" t="str">
+        <f>IF(E19=F19,"Y","N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="45">
+        <v>1</v>
+      </c>
+      <c r="C20" s="45">
+        <v>1</v>
+      </c>
+      <c r="D20" s="46">
+        <f>$G$15+B20*$C$15+C20*$E$15</f>
+        <v>0.5</v>
+      </c>
+      <c r="E20" s="47">
+        <f>IF(D20&lt;0,0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="F20" s="46">
+        <f>OR(B20,C20)*1</f>
+        <v>1</v>
+      </c>
+      <c r="G20" s="33" t="str">
+        <f>IF(E20=F20,"Y","N")</f>
+        <v>Y</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="G2:G7 G9:G14 G16:G20">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
QUIZ passed after 4 weeks almost
</commit_message>
<xml_diff>
--- a/1_ML_Combined_Courses/Practice/4_Excel/2_Simple_Neurons.xlsx
+++ b/1_ML_Combined_Courses/Practice/4_Excel/2_Simple_Neurons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\1_ML_Combined_Courses\Practice\4_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC1A4ED-EDE4-4192-AC03-BA1DA3C678A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110811EA-4F41-4248-A161-039404E97B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{BEFB4AB8-46B2-4D36-AF54-8C400EF49FEA}"/>
   </bookViews>
@@ -434,7 +434,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -577,13 +577,10 @@
     <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -600,7 +597,7 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="2">
     <dxf>
       <font>
         <b/>
@@ -620,30 +617,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2936,7 +2909,7 @@
   <dimension ref="B1:U20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2952,22 +2925,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="55">
-        <v>1</v>
-      </c>
-      <c r="D1" s="55" t="s">
+      <c r="C1" s="54">
+        <v>1</v>
+      </c>
+      <c r="D1" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="55">
-        <v>1</v>
-      </c>
-      <c r="F1" s="56" t="s">
+      <c r="E1" s="54">
+        <v>1</v>
+      </c>
+      <c r="F1" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="57">
+      <c r="G1" s="56">
         <v>-1.5</v>
       </c>
     </row>
@@ -3169,23 +3142,23 @@
       </c>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="55">
+      <c r="C8" s="54">
         <v>-1</v>
       </c>
-      <c r="D8" s="55" t="s">
+      <c r="D8" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="55">
+      <c r="E8" s="54">
         <v>-1</v>
       </c>
-      <c r="F8" s="56" t="s">
+      <c r="F8" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="57">
-        <v>1.5</v>
+      <c r="G8" s="56">
+        <v>0.5</v>
       </c>
       <c r="R8" s="50">
         <v>1</v>
@@ -3240,7 +3213,7 @@
       </c>
       <c r="D10" s="46">
         <f>$G$8+B10*$C$8+C10*$E$8</f>
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="E10" s="47">
         <f>IF(D10&lt;0,0,1)</f>
@@ -3277,11 +3250,11 @@
       </c>
       <c r="D11" s="46">
         <f>$G$8+B11*$C$8+C11*$E$8</f>
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
       <c r="E11" s="47">
         <f>IF(D11&lt;0,0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="46">
         <f>AND(NOT(B11),NOT(C11))*1</f>
@@ -3289,7 +3262,7 @@
       </c>
       <c r="G11" s="33" t="str">
         <f>IF(E11=F11,"Y","N")</f>
-        <v>N</v>
+        <v>Y</v>
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.2">
@@ -3301,11 +3274,11 @@
       </c>
       <c r="D12" s="46">
         <f>$G$8+B12*$C$8+C12*$E$8</f>
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
       <c r="E12" s="47">
         <f>IF(D12&lt;0,0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="46">
         <f>AND(NOT(B12),NOT(C12))*1</f>
@@ -3313,7 +3286,7 @@
       </c>
       <c r="G12" s="33" t="str">
         <f>IF(E12=F12,"Y","N")</f>
-        <v>N</v>
+        <v>Y</v>
       </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.2">
@@ -3325,7 +3298,7 @@
       </c>
       <c r="D13" s="46">
         <f>$G$8+B13*$C$8+C13*$E$8</f>
-        <v>-0.5</v>
+        <v>-1.5</v>
       </c>
       <c r="E13" s="47">
         <f>IF(D13&lt;0,0,1)</f>
@@ -3341,30 +3314,30 @@
       </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B14" s="52"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="53"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="52"/>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B15" s="55" t="s">
+      <c r="B15" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="55">
-        <v>1</v>
-      </c>
-      <c r="D15" s="55" t="s">
+      <c r="C15" s="54">
+        <v>1</v>
+      </c>
+      <c r="D15" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="55">
-        <v>1</v>
-      </c>
-      <c r="F15" s="56" t="s">
+      <c r="E15" s="54">
+        <v>1</v>
+      </c>
+      <c r="F15" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="G15" s="57">
-        <v>-1.5</v>
+      <c r="G15" s="56">
+        <v>-0.5</v>
       </c>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.2">
@@ -3393,7 +3366,7 @@
       </c>
       <c r="D17" s="46">
         <f>$G$15+B17*$C$15+C17*$E$15</f>
-        <v>-1.5</v>
+        <v>-0.5</v>
       </c>
       <c r="E17" s="47">
         <f>IF(D17&lt;0,0,1)</f>
@@ -3417,11 +3390,11 @@
       </c>
       <c r="D18" s="46">
         <f>$G$15+B18*$C$15+C18*$E$15</f>
-        <v>-0.5</v>
+        <v>0.5</v>
       </c>
       <c r="E18" s="47">
         <f>IF(D18&lt;0,0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="46">
         <f>OR(B18,C18)*1</f>
@@ -3429,7 +3402,7 @@
       </c>
       <c r="G18" s="33" t="str">
         <f>IF(E18=F18,"Y","N")</f>
-        <v>N</v>
+        <v>Y</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
@@ -3441,11 +3414,11 @@
       </c>
       <c r="D19" s="46">
         <f>$G$15+B19*$C$15+C19*$E$15</f>
-        <v>-0.5</v>
+        <v>0.5</v>
       </c>
       <c r="E19" s="47">
         <f>IF(D19&lt;0,0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="46">
         <f>OR(B19,C19)*1</f>
@@ -3453,7 +3426,7 @@
       </c>
       <c r="G19" s="33" t="str">
         <f>IF(E19=F19,"Y","N")</f>
-        <v>N</v>
+        <v>Y</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
@@ -3465,7 +3438,7 @@
       </c>
       <c r="D20" s="46">
         <f>$G$15+B20*$C$15+C20*$E$15</f>
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="E20" s="47">
         <f>IF(D20&lt;0,0,1)</f>

</xml_diff>